<commit_message>
Date\time types and styles
</commit_message>
<xml_diff>
--- a/test/xlsx/dateTime.xlsx
+++ b/test/xlsx/dateTime.xlsx
@@ -12,9 +12,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy.mm.dd"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font/>
   </fonts>
@@ -41,9 +39,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf/>
-    <xf numFmtId="164" applyNumberFormat="true"/>
+    <xf numFmtId="14" applyNumberFormat="true"/>
+    <xf numFmtId="21" applyNumberFormat="true"/>
   </cellXfs>
   <dxfs count="0"/>
 </styleSheet>
@@ -51,25 +50,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0" view="normal"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="12" style="1"/>
-    <col min="2" max="2" customWidth="1" width="12" style="1"/>
-    <col min="3" max="3" customWidth="1" width="12" style="1"/>
+    <col min="1" max="1" customWidth="1" width="12"/>
+    <col min="2" max="2" customWidth="1" width="12"/>
+    <col min="3" max="3" customWidth="1" width="12"/>
+    <col min="4" max="4" customWidth="1" width="12"/>
+    <col min="5" max="5" customWidth="1" width="12"/>
+    <col min="6" max="6" customWidth="1" width="12"/>
+    <col min="7" max="7" customWidth="1" width="12"/>
+    <col min="8" max="8" customWidth="1" width="12"/>
+    <col min="9" max="9" customWidth="1" width="12"/>
+    <col min="10" max="10" customWidth="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
         <v>41105.8449537037</v>
       </c>
-      <c r="B1" s="1">
-        <v>42719</v>
+      <c r="B1" s="2">
+        <v>41105.8449537037</v>
       </c>
       <c r="C1" s="1">
-        <v>42719</v>
+        <v>41105.8449537037</v>
+      </c>
+      <c r="D1" s="2">
+        <v>41105.8449537037</v>
+      </c>
+      <c r="E1" s="1">
+        <v>41105.8449537037</v>
+      </c>
+      <c r="F1" s="2">
+        <v>41105.8449537037</v>
+      </c>
+      <c r="G1" s="1">
+        <v>42719.461805555555</v>
+      </c>
+      <c r="H1" s="2">
+        <v>42719.461805555555</v>
+      </c>
+      <c r="I1" s="1">
+        <v>42719.461805555555</v>
+      </c>
+      <c r="J1" s="2">
+        <v>42719.461805555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>